<commit_message>
added if condition to delay at 1st iteration
</commit_message>
<xml_diff>
--- a/Extraction/assets/errors_file.xlsx
+++ b/Extraction/assets/errors_file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="237">
   <x:si>
     <x:t>url</x:t>
   </x:si>
@@ -637,6 +637,165 @@
   </x:si>
   <x:si>
     <x:t>https://www.therealreal.com/products/women/clothing/jackets/patagonia-jacket-fp14g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/pendleton-virgin-wool-biker-jacket-f76bm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/marcell-von-berlin-lambskin-biker-jacket-w-tags-ftm6o</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/capulet-ddusv</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/weekend-max-mara-virgin-wool-jacket-fz2ch</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/sandro-faux-fur-jacket-fr4pn</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/louis-vuitton-2022-damier-azur-denim-jacket-f9iuh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/max-mara-virgin-wool-blazer-ftqa4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/etoile-isabel-marant-tweed-pattern-jacket-fmx6c</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/alberto-makali-fox-fur-jacket-fpnoe</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/zadig-voltaire-floral-print-blazer-fritm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/akris-plaid-print-blazer-fr0i5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/rag-bone-blazer-ftnaw</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/jil-sander-navy-lamb-leather-evening-jacket-frn4l</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/mother-jacket-fnpsq</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/burberry-london-utility-jacket-fmwwh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/diane-von-furstenberg-tweed-pattern-evening-jacket-w-tags-fpftk</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/alice-olivia-printed-faux-fur-jacket-w-tags-fkm2b</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/iro-lamb-fur-printed-fur-jacket-fi5i6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/sprwmn-leather-blazer-fhqws</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/loro-piana-cashmere-blazer-fw9fa</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/hyein-seo-vest-w-tags-fvqyo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/dolce-gabbana-virgin-wool-blazer-fvpt0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/veronica-beard-virgin-wool-blazer-fvfwk</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/veronica-beard-blazer-fve2e</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/akris-punto-jacket-w-tags-fv8uh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/zadig-voltaire-goat-leather-biker-jacket-fv6co</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/st-john-couture-evening-jacket-w-tags-fv6p2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/st-john-couture-patterned-evening-jacket-fv6kd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/michael-kors-collection-virgin-wool-blazer-fuwvh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/apparis-tweed-pattern-jacket-fuvq6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/escada-tweed-pattern-jacket-fw732</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/perfecto-brand-by-schott-nyc-leather-biker-jacket-fw4dw</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/moncler-2016-down-jacket-fw12w</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/reformation-biker-jacket-fvhfy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/burberry-london-evening-jacket-fvg0x</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/rag-bone-plaid-print-faux-fur-jacket-fvfgo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/burberry-london-faux-fur-jacket-fveog</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/marni-evening-jacket-fv3pa</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/vanessa-bruno-faux-fur-jacket-fuwp5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/oscar-de-la-renta-2013-silk-evening-jacket-ftsta</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/etro-floral-print-down-jacket-fthki</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/bisang-alpine-bolero-fr1wb</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/ganni-floral-print-evening-jacket-fpmpl</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/gerard-darel-suede-blazer-fpv5v</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/acne-studios-jacket-fyzfp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/iro-lamb-leather-biker-jacket-w-tags-fm1qq</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/akris-cashmere-blazer-fro0p</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/allsaints-shearling-jacket-fqapb</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/gucci-2019-printed-blazer-fkemu</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/giorgio-armani-blazer-fo0sw</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/valentino-sub-zero-couture-fur-jacket-flx48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/marc-jacobs-colorblock-pattern-bomber-jacket-fv073</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/tory-burch-blazer-fs0np</x:t>
   </x:si>
   <x:si>
     <x:t>UiPath.UIAutomationNext.Exceptions.NodeNotFoundException: Could not find the user-interface (UI) element for this action.
@@ -1012,7 +1171,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B175"/>
+  <x:dimension ref="A1:B233"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
       <x:pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
@@ -2402,52 +2561,476 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="177" spans="1:14">
+    <x:row r="177" spans="1:14" x14ac:dyDescent="0.25">
       <x:c r="A177" s="0" t="s">
         <x:v>177</x:v>
       </x:c>
-      <x:c r="B177" s="3" t="s">
+      <x:c r="B177" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
     </x:row>
-    <x:row r="178" spans="1:14">
+    <x:row r="178" spans="1:14" x14ac:dyDescent="0.25">
       <x:c r="A178" s="0" t="s">
         <x:v>178</x:v>
       </x:c>
-      <x:c r="B178" s="3" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="179" spans="1:14">
+      <x:c r="B178" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="179" spans="1:14" x14ac:dyDescent="0.25">
       <x:c r="A179" s="0" t="s">
         <x:v>179</x:v>
       </x:c>
-      <x:c r="B179" s="3" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="180" spans="1:14">
+      <x:c r="B179" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="180" spans="1:14" x14ac:dyDescent="0.25">
       <x:c r="A180" s="0" t="s">
         <x:v>180</x:v>
       </x:c>
-      <x:c r="B180" s="3" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="181" spans="1:14">
+      <x:c r="B180" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="181" spans="1:14" x14ac:dyDescent="0.25">
       <x:c r="A181" s="0" t="s">
         <x:v>181</x:v>
       </x:c>
-      <x:c r="B181" s="3" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="182" spans="1:14">
+      <x:c r="B181" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="182" spans="1:14" x14ac:dyDescent="0.25">
       <x:c r="A182" s="0" t="s">
         <x:v>182</x:v>
       </x:c>
-      <x:c r="B182" s="3" t="s">
+      <x:c r="B182" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="184" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A184" s="0" t="s">
         <x:v>183</x:v>
+      </x:c>
+      <x:c r="B184" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="185" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A185" s="0" t="s">
+        <x:v>184</x:v>
+      </x:c>
+      <x:c r="B185" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="186" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A186" s="0" t="s">
+        <x:v>185</x:v>
+      </x:c>
+      <x:c r="B186" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="187" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A187" s="0" t="s">
+        <x:v>186</x:v>
+      </x:c>
+      <x:c r="B187" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="188" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A188" s="0" t="s">
+        <x:v>187</x:v>
+      </x:c>
+      <x:c r="B188" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="189" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A189" s="0" t="s">
+        <x:v>188</x:v>
+      </x:c>
+      <x:c r="B189" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="190" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A190" s="0" t="s">
+        <x:v>189</x:v>
+      </x:c>
+      <x:c r="B190" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="191" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A191" s="0" t="s">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="B191" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="192" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A192" s="0" t="s">
+        <x:v>191</x:v>
+      </x:c>
+      <x:c r="B192" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="193" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A193" s="0" t="s">
+        <x:v>192</x:v>
+      </x:c>
+      <x:c r="B193" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="194" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A194" s="0" t="s">
+        <x:v>193</x:v>
+      </x:c>
+      <x:c r="B194" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="195" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A195" s="0" t="s">
+        <x:v>194</x:v>
+      </x:c>
+      <x:c r="B195" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="196" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A196" s="0" t="s">
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="B196" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="197" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A197" s="0" t="s">
+        <x:v>196</x:v>
+      </x:c>
+      <x:c r="B197" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="198" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A198" s="0" t="s">
+        <x:v>197</x:v>
+      </x:c>
+      <x:c r="B198" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="199" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A199" s="0" t="s">
+        <x:v>198</x:v>
+      </x:c>
+      <x:c r="B199" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="200" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A200" s="0" t="s">
+        <x:v>199</x:v>
+      </x:c>
+      <x:c r="B200" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="201" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A201" s="0" t="s">
+        <x:v>200</x:v>
+      </x:c>
+      <x:c r="B201" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="202" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A202" s="0" t="s">
+        <x:v>201</x:v>
+      </x:c>
+      <x:c r="B202" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="203" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A203" s="0" t="s">
+        <x:v>202</x:v>
+      </x:c>
+      <x:c r="B203" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="204" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A204" s="0" t="s">
+        <x:v>203</x:v>
+      </x:c>
+      <x:c r="B204" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="205" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A205" s="0" t="s">
+        <x:v>204</x:v>
+      </x:c>
+      <x:c r="B205" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="206" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A206" s="0" t="s">
+        <x:v>205</x:v>
+      </x:c>
+      <x:c r="B206" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="207" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A207" s="0" t="s">
+        <x:v>206</x:v>
+      </x:c>
+      <x:c r="B207" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="208" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A208" s="0" t="s">
+        <x:v>207</x:v>
+      </x:c>
+      <x:c r="B208" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="209" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A209" s="0" t="s">
+        <x:v>208</x:v>
+      </x:c>
+      <x:c r="B209" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="210" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A210" s="0" t="s">
+        <x:v>209</x:v>
+      </x:c>
+      <x:c r="B210" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="211" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A211" s="0" t="s">
+        <x:v>210</x:v>
+      </x:c>
+      <x:c r="B211" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="212" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A212" s="0" t="s">
+        <x:v>211</x:v>
+      </x:c>
+      <x:c r="B212" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="213" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A213" s="0" t="s">
+        <x:v>212</x:v>
+      </x:c>
+      <x:c r="B213" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="214" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A214" s="0" t="s">
+        <x:v>213</x:v>
+      </x:c>
+      <x:c r="B214" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="215" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A215" s="0" t="s">
+        <x:v>214</x:v>
+      </x:c>
+      <x:c r="B215" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="216" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A216" s="0" t="s">
+        <x:v>215</x:v>
+      </x:c>
+      <x:c r="B216" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="217" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A217" s="0" t="s">
+        <x:v>216</x:v>
+      </x:c>
+      <x:c r="B217" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="218" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A218" s="0" t="s">
+        <x:v>217</x:v>
+      </x:c>
+      <x:c r="B218" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="219" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A219" s="0" t="s">
+        <x:v>218</x:v>
+      </x:c>
+      <x:c r="B219" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="220" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A220" s="0" t="s">
+        <x:v>219</x:v>
+      </x:c>
+      <x:c r="B220" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="221" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A221" s="0" t="s">
+        <x:v>220</x:v>
+      </x:c>
+      <x:c r="B221" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="222" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A222" s="0" t="s">
+        <x:v>221</x:v>
+      </x:c>
+      <x:c r="B222" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="223" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A223" s="0" t="s">
+        <x:v>222</x:v>
+      </x:c>
+      <x:c r="B223" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="224" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A224" s="0" t="s">
+        <x:v>223</x:v>
+      </x:c>
+      <x:c r="B224" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="225" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A225" s="0" t="s">
+        <x:v>224</x:v>
+      </x:c>
+      <x:c r="B225" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="226" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A226" s="0" t="s">
+        <x:v>225</x:v>
+      </x:c>
+      <x:c r="B226" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="227" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A227" s="0" t="s">
+        <x:v>226</x:v>
+      </x:c>
+      <x:c r="B227" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="228" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A228" s="0" t="s">
+        <x:v>227</x:v>
+      </x:c>
+      <x:c r="B228" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="229" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A229" s="0" t="s">
+        <x:v>228</x:v>
+      </x:c>
+      <x:c r="B229" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="230" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A230" s="0" t="s">
+        <x:v>229</x:v>
+      </x:c>
+      <x:c r="B230" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="231" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A231" s="0" t="s">
+        <x:v>230</x:v>
+      </x:c>
+      <x:c r="B231" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="232" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A232" s="0" t="s">
+        <x:v>231</x:v>
+      </x:c>
+      <x:c r="B232" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="233" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A233" s="0" t="s">
+        <x:v>232</x:v>
+      </x:c>
+      <x:c r="B233" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="235" spans="1:14">
+      <x:c r="A235" s="0" t="s">
+        <x:v>233</x:v>
+      </x:c>
+      <x:c r="B235" s="3" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="236" spans="1:14">
+      <x:c r="A236" s="0" t="s">
+        <x:v>234</x:v>
+      </x:c>
+      <x:c r="B236" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="237" spans="1:14">
+      <x:c r="A237" s="0" t="s">
+        <x:v>235</x:v>
+      </x:c>
+      <x:c r="B237" s="3" t="s">
+        <x:v>236</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
ad rec moving and this will be cloned to other lap
</commit_message>
<xml_diff>
--- a/Extraction/assets/errors_file.xlsx
+++ b/Extraction/assets/errors_file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1969" uniqueCount="1969">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2083" uniqueCount="2083">
   <x:si>
     <x:t>url</x:t>
   </x:si>
@@ -6056,6 +6056,348 @@
   </x:si>
   <x:si>
     <x:t>https://www.therealreal.com/products/women/clothing/tops/doen-bateau-neckline-three-quarter-sleeve-crop-top-fd326</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/shoes/sandals/chanel-vintage-tweed-pattern-slingback-sandals-fzwmv</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/handbags/totes/chanel-caviar-medallion-tote-fym5f</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/handbags/totes/louis-vuitton-antigua-cabas-gm-fzuif</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/pants/yves-saint-laurent-rive-gauche-vintage-wide-leg-pants-fxu1h</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/handbags/handle-bags/fendi-vintage-mini-pochette-g0akv</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/accessories/belts/chanel-vintage-2005-waist-belt-g0mye</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/accessories/belts/chanel-vintage-1990-chain-link-belt-fx0q4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/coats/chanel-vintage-2002-fur-coat-fy8lb</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/coats/valentino-vintage-2000-s-down-coat-fynfh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/tops/jean-paul-gaultier-vintage-2004-tunic-g0se7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/skirts/d-g-vintage-mini-skirt-frh3u</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/accessories/wallets/chanel-vintage-2006-2008-compact-wallet-fw9d6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/coats/burberry-s-vintage-trench-coat-fywzu</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/handbags/handle-bags/louis-vuitton-vintage-monogram-ellipse-pm-fm1dq</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/skirts/gucci-vintage-midi-length-skirt-fl3ri</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/suits-and-sets/issey-miyake-vintage-late-1980-s-early-1990-s-skirt-set-ftndc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/pants/gianni-versace-vintage-straight-leg-pants-e8qk5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/dolce-gabbana-vintage-late-1990-s-early-2000-s-fur-jacket-e4xas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/bath-and-body/body-oils/everyday-oil-mainstay-blend-8-oz-dk50r</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/bath-and-body/body-wash/joanna-vargas-vitamin-c-face-wash-enk76</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/skincare/tools-and-accessories/well-kept-exfoliating-washcloth-e97f4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/bath-and-body/hand-soap-and-moisturizers/grown-alchemist-hand-wash-sweet-orange-cedarwood-sage-300ml-eo44i</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/bath-and-body/hand-soap-and-moisturizers/nopalera-cactus-soap-in-planta-futura-e2wc7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/hair-care/shampoo-and-conditioner/ceremonia-guava-rescue-spray-dgdke</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/fragrance/spicy/boy-smells-cowboy-kush-eau-de-parfum-etg55</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/fragrance/spicy/boy-smells-hinoki-fantome-eau-de-parfum-etfvo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/makeup/lips/henne-organics-desire-luxury-lip-tint-elhwk</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/makeup/lips/henne-organics-bare-luxury-lip-tint-elhyb</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/makeup/lips/henne-organics-muse-luxury-lip-tint-elht2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/skincare/tools-and-accessories/lanshin-rose-quartz-sculpting-spoon-eml2z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/makeup/lips/henne-organics-intrigue-luxury-lip-tint-elhv2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/hair-care/brushes-and-combs/machete-no-4-comb-orchid-ekry2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/skincare/ubeauty-resurfacing-compound-adrj9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/makeup/lips/dr-devgan-platinum-lip-plump-spf-30-do7mw</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/fragrance/woody/cra-yon-sand-service-50ml-eau-de-parfum-ef3ve</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/fragrance/fresh/cra-yon-vanilla-ceo-50ml-eau-de-parfum-ef3su</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/skincare/masks-and-exfoliators/nopalera-cactus-flower-exfoliant-e2wa6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/bath-and-body/body-moisturizers/lauren-s-all-purpose-classic-jar-e6p57</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/skincare/serums/joanna-vargas-rescue-serum-ah655</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/bath-and-body/body-wash/corpus-natural-body-wash-no-green-c9kmq</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/bath-and-body/hand-soap-and-moisturizers/nopalera-cactus-soap-in-flor-de-mayo-e2wbx</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/fragrance/spicy/19-69-chinese-tobacco-eau-de-parfum-bjpbe</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/skincare/joanna-vargas-daily-serum-9szi8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/fragrance/woody/19-69-rainbow-bar-eau-de-parfum-bjqcn</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/hair-care/hair-masks/ceremonia-pequi-curl-activator-200ml-e4nbv</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/bath-and-body/mason-pearson-popular-mixture-hair-brush-c7ilb</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/skincare/face-oils/rowse-rosehip-oil-dt2o3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/bath-and-body/body-oils/kindred-black-a-woman-is-fire-all-natural-perfume-dk4r8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/bath-and-body/hand-soap-and-moisturizers/claus-porto-gift-box-9-deco-soaps-c7j30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/skincare/masks-and-exfoliators/knc-beauty-star-eye-mask-set-dan7g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/hair-care/crown-affair-scrunchie-no-001-pack-of-3-do7rh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/skincare/face-oils/mara-algae-moringa-universal-face-oil-adv37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/skincare/masks-and-exfoliators/joanna-vargas-forever-glow-anti-aging-face-mask-anmgs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/skincare/tools-and-accessories/sounds-gua-sha-rose-quartz-doj67</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/makeup/lips/henne-organics-bare-luxury-lip-tint-c9ixw</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/hair-care/shampoo-and-conditioner/ceremonia-champu-de-yucca-witch-hazel-dgdns</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/hair-care/shampoo-and-conditioner/ceremonia-guava-leave-in-conditioner-dgdfw</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/skincare/moisturizers/ubeauty-the-super-smart-hydrator-adlq7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/makeup/face/saie-sunglow-glowy-super-gel-luminizer-cph58</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/hair-care/brushes-and-combs/crown-affair-brush-no-001-c9j4f</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/bath-and-body/body-wash/austin-austin-neroli-petitgrain-body-soap-ag1yl</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/makeup/olio-e-osso-balm-no-3-crimson-adpys</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/fragrance/ormaie-l-ivree-bleue-edp-50ml-c4deb</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/bath-and-body/body-wash/corpus-natural-body-wash-third-rose-c9k6c</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/makeup/face/saie-dreamy-liquid-blush-cph6d</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/skincare/tools-and-accessories/gilded-body-the-marble-body-brush-calacatta-viola-d8yk7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/skincare/tools-and-accessories/gilded-body-the-marble-body-brush-lichen-flower-d8yo5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/hair-care/brushes-and-combs/crown-affair-the-comb-no-002-d7cr7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/hair-care/hair-masks/crown-affair-the-renewal-mask-d7cuo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/bath-and-body/hand-soap-and-moisturizers/austin-austin-palmarosa-vetiver-hand-soap-c9kru</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/fragrance/fresh/d-s-durga-i-don-t-know-what-eau-de-parfum-100ml-ci9r9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/fragrance/fresh/d-s-durga-i-don-t-know-what-eau-de-parfum-50ml-cia1y</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/fragrance/floral/d-s-durga-jazmin-yucatan-eau-de-parfum-50ml-ci9z2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/makeup/face/saie-rosy-liquid-blush-cphs2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/makeup/face/saie-the-big-makeup-brush-cpgi8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/makeup/face/saie-starglow-glowy-super-gel-luminizer-cpife</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/makeup/lips/henne-organics-desire-luxury-lip-tint-d371r</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/fragrance/floral/regime-des-fleurs-chloe-sevigny-little-flower-eau-de-parfum-ca6e3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/fragrance/woody/d-s-durga-debaser-pocket-perfume-cxoi5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/bath-and-body/body-wash/flamingo-estate-body-wash-ci6bw</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/skincare/moisturizers/kindred-black-damiana-aphrodisiac-lip-skin-balm-cibes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/hair-care/brushes-and-combs/crown-affair-the-comb-no-001-ck67i</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/beauty/hair-care/brushes-and-combs/crown-affair-the-comb-no-002-bzc9c</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/accessories/hats/prada-puffer-trapper-hat-elj8v</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/accessories/sunglasses/jeremy-scott-x-linda-farrow-shield-tinted-sunglasses-eu3m0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/coats/vetements-down-coat-w-tags-bvn4p</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jumpsuits-and-rompers/emilio-pucci-vintage-late-1960-s-early-1970-s-jumpsuit-esw9y</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/accessories/winter-accessories/prada-woven-gloves-eodj2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/accessories/hats/bogner-embroidered-ski-hat-e6m69</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/accessories/scarves-and-shawls/loewe-paula-s-ibiza-printed-scarf-evl4a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/bottega-veneta-down-jacket-fyvl7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/accessories/sunglasses/celine-vintage-shield-sunglasses-foza1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/shoes/boots/louis-vuitton-pillow-comfort-lv-monogram-snow-boots-d60xd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/the-north-face-jacket-g1o2t</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/home/sports/snow-gear/burton-family-tree-straight-chuter-camber-splitboard-cnw30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/stand-studio-down-jacket-w-tags-ez7dh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/coats/chanel-vintage-1990-performance-coat-fku5t</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/accessories/sunglasses/cartier-oversize-tinted-sunglasses-f1kvq</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/accessories/winter-accessories/saint-laurent-leather-winter-gloves-g1j91</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/knitwear/fendi-v-neck-sweater-fusdc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/accessories/hats/chanel-wool-beanie-w-tags-ff4cw</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/accessories/winter-accessories/celine-winter-gloves-ff9gl</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/handbags/luggage-and-travel/louis-vuitton-monogram-summer-trunks-keepall-bandouliere-50-djox5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/emilio-pucci-vintage-2000-s-jacket-fyr4w</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/accessories/hats/chanel-2022-cashmere-cc-beanie-w-tags-funzo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/accessories/hats/the-elder-statesman-cashmere-beanie-fxtpd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/accessories/scarves-and-shawls/hermes-casaque-optique-cashmere-muffler-fw3vj</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/handbags/backpacks/chanel-coco-neige-shearling-backpack-erpye</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/tops/eckhaus-latta-floral-print-turtleneck-crop-top-g126o</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/accessories/scarves-and-shawls/prada-nylon-printed-scarf-fsqfz</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/accessories/sunglasses/celine-shield-gradient-sunglasses-g0y15</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/clothing/jackets/moncler-grenoble-houndstooth-print-down-jacket-fzr4v</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/home/sports/snow-gear/head-wc-rebels-racing-skis-c7brq</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.therealreal.com/products/women/accessories/winter-accessories/chanel-2020-cashmere-fingerless-gloves-w-tags-ftvep</x:t>
   </x:si>
   <x:si>
     <x:t>UiPath.UIAutomationNext.Exceptions.NodeNotFoundException: Could not find the user-interface (UI) element for this action.
@@ -22674,7 +23016,919 @@
         <x:v>1967</x:v>
       </x:c>
       <x:c r="B2032" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2034" spans="1:14">
+      <x:c r="A2034" s="0" t="s">
         <x:v>1968</x:v>
+      </x:c>
+      <x:c r="B2034" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2035" spans="1:14">
+      <x:c r="A2035" s="0" t="s">
+        <x:v>1969</x:v>
+      </x:c>
+      <x:c r="B2035" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2036" spans="1:14">
+      <x:c r="A2036" s="0" t="s">
+        <x:v>1970</x:v>
+      </x:c>
+      <x:c r="B2036" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2037" spans="1:14">
+      <x:c r="A2037" s="0" t="s">
+        <x:v>1971</x:v>
+      </x:c>
+      <x:c r="B2037" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2038" spans="1:14">
+      <x:c r="A2038" s="0" t="s">
+        <x:v>1972</x:v>
+      </x:c>
+      <x:c r="B2038" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2039" spans="1:14">
+      <x:c r="A2039" s="0" t="s">
+        <x:v>1973</x:v>
+      </x:c>
+      <x:c r="B2039" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2040" spans="1:14">
+      <x:c r="A2040" s="0" t="s">
+        <x:v>1974</x:v>
+      </x:c>
+      <x:c r="B2040" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2041" spans="1:14">
+      <x:c r="A2041" s="0" t="s">
+        <x:v>1975</x:v>
+      </x:c>
+      <x:c r="B2041" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2042" spans="1:14">
+      <x:c r="A2042" s="0" t="s">
+        <x:v>1976</x:v>
+      </x:c>
+      <x:c r="B2042" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2043" spans="1:14">
+      <x:c r="A2043" s="0" t="s">
+        <x:v>1977</x:v>
+      </x:c>
+      <x:c r="B2043" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2044" spans="1:14">
+      <x:c r="A2044" s="0" t="s">
+        <x:v>1978</x:v>
+      </x:c>
+      <x:c r="B2044" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2045" spans="1:14">
+      <x:c r="A2045" s="0" t="s">
+        <x:v>1979</x:v>
+      </x:c>
+      <x:c r="B2045" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2046" spans="1:14">
+      <x:c r="A2046" s="0" t="s">
+        <x:v>1980</x:v>
+      </x:c>
+      <x:c r="B2046" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2047" spans="1:14">
+      <x:c r="A2047" s="0" t="s">
+        <x:v>1981</x:v>
+      </x:c>
+      <x:c r="B2047" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2048" spans="1:14">
+      <x:c r="A2048" s="0" t="s">
+        <x:v>1982</x:v>
+      </x:c>
+      <x:c r="B2048" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2049" spans="1:14">
+      <x:c r="A2049" s="0" t="s">
+        <x:v>1983</x:v>
+      </x:c>
+      <x:c r="B2049" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2050" spans="1:14">
+      <x:c r="A2050" s="0" t="s">
+        <x:v>1984</x:v>
+      </x:c>
+      <x:c r="B2050" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2051" spans="1:14">
+      <x:c r="A2051" s="0" t="s">
+        <x:v>1985</x:v>
+      </x:c>
+      <x:c r="B2051" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2053" spans="1:14">
+      <x:c r="A2053" s="0" t="s">
+        <x:v>1986</x:v>
+      </x:c>
+      <x:c r="B2053" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2054" spans="1:14">
+      <x:c r="A2054" s="0" t="s">
+        <x:v>1987</x:v>
+      </x:c>
+      <x:c r="B2054" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2056" spans="1:14">
+      <x:c r="A2056" s="0" t="s">
+        <x:v>1988</x:v>
+      </x:c>
+      <x:c r="B2056" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2057" spans="1:14">
+      <x:c r="A2057" s="0" t="s">
+        <x:v>1989</x:v>
+      </x:c>
+      <x:c r="B2057" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2058" spans="1:14">
+      <x:c r="A2058" s="0" t="s">
+        <x:v>1990</x:v>
+      </x:c>
+      <x:c r="B2058" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2059" spans="1:14">
+      <x:c r="A2059" s="0" t="s">
+        <x:v>1991</x:v>
+      </x:c>
+      <x:c r="B2059" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2060" spans="1:14">
+      <x:c r="A2060" s="0" t="s">
+        <x:v>1992</x:v>
+      </x:c>
+      <x:c r="B2060" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2061" spans="1:14">
+      <x:c r="A2061" s="0" t="s">
+        <x:v>1993</x:v>
+      </x:c>
+      <x:c r="B2061" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2062" spans="1:14">
+      <x:c r="A2062" s="0" t="s">
+        <x:v>1994</x:v>
+      </x:c>
+      <x:c r="B2062" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2063" spans="1:14">
+      <x:c r="A2063" s="0" t="s">
+        <x:v>1995</x:v>
+      </x:c>
+      <x:c r="B2063" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2064" spans="1:14">
+      <x:c r="A2064" s="0" t="s">
+        <x:v>1996</x:v>
+      </x:c>
+      <x:c r="B2064" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2065" spans="1:14">
+      <x:c r="A2065" s="0" t="s">
+        <x:v>1997</x:v>
+      </x:c>
+      <x:c r="B2065" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2066" spans="1:14">
+      <x:c r="A2066" s="0" t="s">
+        <x:v>1998</x:v>
+      </x:c>
+      <x:c r="B2066" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2067" spans="1:14">
+      <x:c r="A2067" s="0" t="s">
+        <x:v>1999</x:v>
+      </x:c>
+      <x:c r="B2067" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2068" spans="1:14">
+      <x:c r="A2068" s="0" t="s">
+        <x:v>2000</x:v>
+      </x:c>
+      <x:c r="B2068" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2069" spans="1:14">
+      <x:c r="A2069" s="0" t="s">
+        <x:v>2001</x:v>
+      </x:c>
+      <x:c r="B2069" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2070" spans="1:14">
+      <x:c r="A2070" s="0" t="s">
+        <x:v>2002</x:v>
+      </x:c>
+      <x:c r="B2070" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2071" spans="1:14">
+      <x:c r="A2071" s="0" t="s">
+        <x:v>2003</x:v>
+      </x:c>
+      <x:c r="B2071" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2072" spans="1:14">
+      <x:c r="A2072" s="0" t="s">
+        <x:v>2004</x:v>
+      </x:c>
+      <x:c r="B2072" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2073" spans="1:14">
+      <x:c r="A2073" s="0" t="s">
+        <x:v>2005</x:v>
+      </x:c>
+      <x:c r="B2073" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2074" spans="1:14">
+      <x:c r="A2074" s="0" t="s">
+        <x:v>2006</x:v>
+      </x:c>
+      <x:c r="B2074" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2075" spans="1:14">
+      <x:c r="A2075" s="0" t="s">
+        <x:v>2007</x:v>
+      </x:c>
+      <x:c r="B2075" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2076" spans="1:14">
+      <x:c r="A2076" s="0" t="s">
+        <x:v>2008</x:v>
+      </x:c>
+      <x:c r="B2076" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2077" spans="1:14">
+      <x:c r="A2077" s="0" t="s">
+        <x:v>2009</x:v>
+      </x:c>
+      <x:c r="B2077" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2078" spans="1:14">
+      <x:c r="A2078" s="0" t="s">
+        <x:v>2010</x:v>
+      </x:c>
+      <x:c r="B2078" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2079" spans="1:14">
+      <x:c r="A2079" s="0" t="s">
+        <x:v>2011</x:v>
+      </x:c>
+      <x:c r="B2079" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2080" spans="1:14">
+      <x:c r="A2080" s="0" t="s">
+        <x:v>2012</x:v>
+      </x:c>
+      <x:c r="B2080" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2081" spans="1:14">
+      <x:c r="A2081" s="0" t="s">
+        <x:v>2013</x:v>
+      </x:c>
+      <x:c r="B2081" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2082" spans="1:14">
+      <x:c r="A2082" s="0" t="s">
+        <x:v>2014</x:v>
+      </x:c>
+      <x:c r="B2082" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2083" spans="1:14">
+      <x:c r="A2083" s="0" t="s">
+        <x:v>2015</x:v>
+      </x:c>
+      <x:c r="B2083" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2084" spans="1:14">
+      <x:c r="A2084" s="0" t="s">
+        <x:v>2016</x:v>
+      </x:c>
+      <x:c r="B2084" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2085" spans="1:14">
+      <x:c r="A2085" s="0" t="s">
+        <x:v>2017</x:v>
+      </x:c>
+      <x:c r="B2085" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2086" spans="1:14">
+      <x:c r="A2086" s="0" t="s">
+        <x:v>2018</x:v>
+      </x:c>
+      <x:c r="B2086" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2087" spans="1:14">
+      <x:c r="A2087" s="0" t="s">
+        <x:v>2019</x:v>
+      </x:c>
+      <x:c r="B2087" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2088" spans="1:14">
+      <x:c r="A2088" s="0" t="s">
+        <x:v>2020</x:v>
+      </x:c>
+      <x:c r="B2088" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2089" spans="1:14">
+      <x:c r="A2089" s="0" t="s">
+        <x:v>2021</x:v>
+      </x:c>
+      <x:c r="B2089" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2090" spans="1:14">
+      <x:c r="A2090" s="0" t="s">
+        <x:v>2022</x:v>
+      </x:c>
+      <x:c r="B2090" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2091" spans="1:14">
+      <x:c r="A2091" s="0" t="s">
+        <x:v>2023</x:v>
+      </x:c>
+      <x:c r="B2091" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2092" spans="1:14">
+      <x:c r="A2092" s="0" t="s">
+        <x:v>2024</x:v>
+      </x:c>
+      <x:c r="B2092" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2093" spans="1:14">
+      <x:c r="A2093" s="0" t="s">
+        <x:v>2025</x:v>
+      </x:c>
+      <x:c r="B2093" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2094" spans="1:14">
+      <x:c r="A2094" s="0" t="s">
+        <x:v>2026</x:v>
+      </x:c>
+      <x:c r="B2094" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2095" spans="1:14">
+      <x:c r="A2095" s="0" t="s">
+        <x:v>2027</x:v>
+      </x:c>
+      <x:c r="B2095" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2096" spans="1:14">
+      <x:c r="A2096" s="0" t="s">
+        <x:v>2028</x:v>
+      </x:c>
+      <x:c r="B2096" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2097" spans="1:14">
+      <x:c r="A2097" s="0" t="s">
+        <x:v>2029</x:v>
+      </x:c>
+      <x:c r="B2097" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2098" spans="1:14">
+      <x:c r="A2098" s="0" t="s">
+        <x:v>2030</x:v>
+      </x:c>
+      <x:c r="B2098" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2099" spans="1:14">
+      <x:c r="A2099" s="0" t="s">
+        <x:v>2031</x:v>
+      </x:c>
+      <x:c r="B2099" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2100" spans="1:14">
+      <x:c r="A2100" s="0" t="s">
+        <x:v>2032</x:v>
+      </x:c>
+      <x:c r="B2100" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2101" spans="1:14">
+      <x:c r="A2101" s="0" t="s">
+        <x:v>2033</x:v>
+      </x:c>
+      <x:c r="B2101" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2102" spans="1:14">
+      <x:c r="A2102" s="0" t="s">
+        <x:v>2034</x:v>
+      </x:c>
+      <x:c r="B2102" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2103" spans="1:14">
+      <x:c r="A2103" s="0" t="s">
+        <x:v>2035</x:v>
+      </x:c>
+      <x:c r="B2103" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2104" spans="1:14">
+      <x:c r="A2104" s="0" t="s">
+        <x:v>2036</x:v>
+      </x:c>
+      <x:c r="B2104" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2105" spans="1:14">
+      <x:c r="A2105" s="0" t="s">
+        <x:v>2037</x:v>
+      </x:c>
+      <x:c r="B2105" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2106" spans="1:14">
+      <x:c r="A2106" s="0" t="s">
+        <x:v>2038</x:v>
+      </x:c>
+      <x:c r="B2106" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2107" spans="1:14">
+      <x:c r="A2107" s="0" t="s">
+        <x:v>2039</x:v>
+      </x:c>
+      <x:c r="B2107" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2108" spans="1:14">
+      <x:c r="A2108" s="0" t="s">
+        <x:v>2040</x:v>
+      </x:c>
+      <x:c r="B2108" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2109" spans="1:14">
+      <x:c r="A2109" s="0" t="s">
+        <x:v>2041</x:v>
+      </x:c>
+      <x:c r="B2109" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2110" spans="1:14">
+      <x:c r="A2110" s="0" t="s">
+        <x:v>2042</x:v>
+      </x:c>
+      <x:c r="B2110" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2111" spans="1:14">
+      <x:c r="A2111" s="0" t="s">
+        <x:v>2043</x:v>
+      </x:c>
+      <x:c r="B2111" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2112" spans="1:14">
+      <x:c r="A2112" s="0" t="s">
+        <x:v>2044</x:v>
+      </x:c>
+      <x:c r="B2112" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2113" spans="1:14">
+      <x:c r="A2113" s="0" t="s">
+        <x:v>2045</x:v>
+      </x:c>
+      <x:c r="B2113" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2114" spans="1:14">
+      <x:c r="A2114" s="0" t="s">
+        <x:v>2046</x:v>
+      </x:c>
+      <x:c r="B2114" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2115" spans="1:14">
+      <x:c r="A2115" s="0" t="s">
+        <x:v>2047</x:v>
+      </x:c>
+      <x:c r="B2115" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2116" spans="1:14">
+      <x:c r="A2116" s="0" t="s">
+        <x:v>2048</x:v>
+      </x:c>
+      <x:c r="B2116" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2117" spans="1:14">
+      <x:c r="A2117" s="0" t="s">
+        <x:v>2049</x:v>
+      </x:c>
+      <x:c r="B2117" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2118" spans="1:14">
+      <x:c r="A2118" s="0" t="s">
+        <x:v>2050</x:v>
+      </x:c>
+      <x:c r="B2118" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2120" spans="1:14">
+      <x:c r="A2120" s="0" t="s">
+        <x:v>2051</x:v>
+      </x:c>
+      <x:c r="B2120" s="3" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2121" spans="1:14">
+      <x:c r="A2121" s="0" t="s">
+        <x:v>2052</x:v>
+      </x:c>
+      <x:c r="B2121" s="3" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2122" spans="1:14">
+      <x:c r="A2122" s="0" t="s">
+        <x:v>2053</x:v>
+      </x:c>
+      <x:c r="B2122" s="3" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2123" spans="1:14">
+      <x:c r="A2123" s="0" t="s">
+        <x:v>2054</x:v>
+      </x:c>
+      <x:c r="B2123" s="3" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2124" spans="1:14">
+      <x:c r="A2124" s="0" t="s">
+        <x:v>2055</x:v>
+      </x:c>
+      <x:c r="B2124" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2125" spans="1:14">
+      <x:c r="A2125" s="0" t="s">
+        <x:v>2056</x:v>
+      </x:c>
+      <x:c r="B2125" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2126" spans="1:14">
+      <x:c r="A2126" s="0" t="s">
+        <x:v>2057</x:v>
+      </x:c>
+      <x:c r="B2126" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2127" spans="1:14">
+      <x:c r="A2127" s="0" t="s">
+        <x:v>2058</x:v>
+      </x:c>
+      <x:c r="B2127" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2128" spans="1:14">
+      <x:c r="A2128" s="0" t="s">
+        <x:v>2059</x:v>
+      </x:c>
+      <x:c r="B2128" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2130" spans="1:14">
+      <x:c r="A2130" s="0" t="s">
+        <x:v>2060</x:v>
+      </x:c>
+      <x:c r="B2130" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2131" spans="1:14">
+      <x:c r="A2131" s="0" t="s">
+        <x:v>2061</x:v>
+      </x:c>
+      <x:c r="B2131" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2132" spans="1:14">
+      <x:c r="A2132" s="0" t="s">
+        <x:v>2062</x:v>
+      </x:c>
+      <x:c r="B2132" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2133" spans="1:14">
+      <x:c r="A2133" s="0" t="s">
+        <x:v>2063</x:v>
+      </x:c>
+      <x:c r="B2133" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2134" spans="1:14">
+      <x:c r="A2134" s="0" t="s">
+        <x:v>2064</x:v>
+      </x:c>
+      <x:c r="B2134" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2135" spans="1:14">
+      <x:c r="A2135" s="0" t="s">
+        <x:v>2065</x:v>
+      </x:c>
+      <x:c r="B2135" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2136" spans="1:14">
+      <x:c r="A2136" s="0" t="s">
+        <x:v>2066</x:v>
+      </x:c>
+      <x:c r="B2136" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2137" spans="1:14">
+      <x:c r="A2137" s="0" t="s">
+        <x:v>2067</x:v>
+      </x:c>
+      <x:c r="B2137" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2138" spans="1:14">
+      <x:c r="A2138" s="0" t="s">
+        <x:v>2068</x:v>
+      </x:c>
+      <x:c r="B2138" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2139" spans="1:14">
+      <x:c r="A2139" s="0" t="s">
+        <x:v>2069</x:v>
+      </x:c>
+      <x:c r="B2139" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2140" spans="1:14">
+      <x:c r="A2140" s="0" t="s">
+        <x:v>2070</x:v>
+      </x:c>
+      <x:c r="B2140" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2141" spans="1:14">
+      <x:c r="A2141" s="0" t="s">
+        <x:v>2071</x:v>
+      </x:c>
+      <x:c r="B2141" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2142" spans="1:14">
+      <x:c r="A2142" s="0" t="s">
+        <x:v>2072</x:v>
+      </x:c>
+      <x:c r="B2142" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2143" spans="1:14">
+      <x:c r="A2143" s="0" t="s">
+        <x:v>2073</x:v>
+      </x:c>
+      <x:c r="B2143" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2144" spans="1:14">
+      <x:c r="A2144" s="0" t="s">
+        <x:v>2074</x:v>
+      </x:c>
+      <x:c r="B2144" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2145" spans="1:14">
+      <x:c r="A2145" s="0" t="s">
+        <x:v>2075</x:v>
+      </x:c>
+      <x:c r="B2145" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2146" spans="1:14">
+      <x:c r="A2146" s="0" t="s">
+        <x:v>2076</x:v>
+      </x:c>
+      <x:c r="B2146" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2147" spans="1:14">
+      <x:c r="A2147" s="0" t="s">
+        <x:v>2077</x:v>
+      </x:c>
+      <x:c r="B2147" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2148" spans="1:14">
+      <x:c r="A2148" s="0" t="s">
+        <x:v>2078</x:v>
+      </x:c>
+      <x:c r="B2148" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2149" spans="1:14">
+      <x:c r="A2149" s="0" t="s">
+        <x:v>2079</x:v>
+      </x:c>
+      <x:c r="B2149" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2150" spans="1:14">
+      <x:c r="A2150" s="0" t="s">
+        <x:v>2080</x:v>
+      </x:c>
+      <x:c r="B2150" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2151" spans="1:14">
+      <x:c r="A2151" s="0" t="s">
+        <x:v>2081</x:v>
+      </x:c>
+      <x:c r="B2151" s="3" t="s">
+        <x:v>2082</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>